<commit_message>
Added rational to matrix
Requirement #3 asks for a description of the method and rationale for our values, so I just added a paragraph at the bottom.
</commit_message>
<xml_diff>
--- a/Decision Matrix.xlsx
+++ b/Decision Matrix.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Desktop\ECE411\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Project Proposal</t>
   </si>
@@ -135,16 +130,22 @@
   </si>
   <si>
     <t>Motors</t>
+  </si>
+  <si>
+    <t>Rationale:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We chose complexity and creativity to be weighted the highest. Complexity is important because we don't want to hit "the wall" or reach "the cliff" that might prevent us from completing the project. Creativity is important because that implies that we would have more opportunity to work with a wider variety and more unique components. We chose price and size to be low-moderate weighting because the size requirements should be easy to meet, and we don't feel like it's very probable that we are forced into buying expensive parts. Lastly, soldering difficulty is weighted low becuase we don't mind the challenge, and we don't anticipate being forced to solder anything particularly difficult. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -414,21 +424,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -438,6 +433,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -492,8 +499,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -556,7 +572,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -608,7 +624,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -802,55 +818,55 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="1.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="1.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="1.875" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="1.875" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="16.125" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="23.45" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="15"/>
+      <c r="F1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="40"/>
       <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
@@ -870,11 +886,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:13" ht="15.75" thickTop="1">
+      <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="6">
@@ -895,26 +911,26 @@
       <c r="H2" s="10">
         <v>3</v>
       </c>
-      <c r="I2" s="32">
-        <v>3</v>
-      </c>
-      <c r="J2" s="29">
-        <v>3</v>
-      </c>
-      <c r="K2" s="20">
+      <c r="I2" s="31">
+        <v>3</v>
+      </c>
+      <c r="J2" s="28">
+        <v>3</v>
+      </c>
+      <c r="K2" s="15">
         <v>1</v>
       </c>
-      <c r="L2" s="20">
-        <v>2</v>
-      </c>
-      <c r="M2" s="20">
+      <c r="L2" s="15">
+        <v>2</v>
+      </c>
+      <c r="M2" s="15">
         <f>-SUM(E2:E4)*$E$15-SUM(H2:H4)*$H$15+I2*$I$15+J2*$J$15+K2*$K$15+L2*$L$15</f>
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
-      <c r="B3" s="24"/>
+    <row r="3" spans="1:13">
+      <c r="A3" s="20"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="8">
         <v>2</v>
       </c>
@@ -929,15 +945,15 @@
       <c r="H3" s="11">
         <v>2</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="25"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A4" s="21"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="2">
         <v>3</v>
       </c>
@@ -948,17 +964,17 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="33"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickTop="1">
       <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="8">
@@ -979,26 +995,26 @@
       <c r="H5" s="11">
         <v>1</v>
       </c>
-      <c r="I5" s="32">
-        <v>3</v>
-      </c>
-      <c r="J5" s="38">
-        <v>2</v>
-      </c>
-      <c r="K5" s="41">
-        <v>3</v>
-      </c>
-      <c r="L5" s="41">
+      <c r="I5" s="31">
+        <v>3</v>
+      </c>
+      <c r="J5" s="37">
+        <v>2</v>
+      </c>
+      <c r="K5" s="18">
+        <v>3</v>
+      </c>
+      <c r="L5" s="18">
         <v>4</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="15">
         <f t="shared" ref="M5" si="0">-SUM(E5:E7)*$E$15-SUM(H5:H7)*$H$15+I5*$I$15+J5*$J$15+K5*$K$15+L5*$L$15</f>
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="24"/>
+    <row r="6" spans="1:13">
+      <c r="A6" s="20"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="8">
         <v>2</v>
       </c>
@@ -1013,15 +1029,15 @@
       <c r="H6" s="11">
         <v>3</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2">
         <v>3</v>
       </c>
@@ -1032,17 +1048,17 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="33"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="8">
@@ -1063,26 +1079,26 @@
       <c r="H8" s="11">
         <v>3</v>
       </c>
-      <c r="I8" s="35">
-        <v>3</v>
-      </c>
-      <c r="J8" s="38">
-        <v>3</v>
-      </c>
-      <c r="K8" s="41">
-        <v>2</v>
-      </c>
-      <c r="L8" s="41">
-        <v>3</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="I8" s="34">
+        <v>3</v>
+      </c>
+      <c r="J8" s="37">
+        <v>3</v>
+      </c>
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>3</v>
+      </c>
+      <c r="M8" s="15">
         <f t="shared" ref="M8" si="1">-SUM(E8:E10)*$E$15-SUM(H8:H10)*$H$15+I8*$I$15+J8*$J$15+K8*$K$15+L8*$L$15</f>
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="24"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="20"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="8">
         <v>2</v>
       </c>
@@ -1101,15 +1117,15 @@
       <c r="H9" s="11">
         <v>1</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="25"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2">
         <v>3</v>
       </c>
@@ -1120,17 +1136,17 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="36"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickTop="1">
       <c r="A11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="8">
@@ -1151,26 +1167,26 @@
       <c r="H11" s="11">
         <v>3</v>
       </c>
-      <c r="I11" s="35">
-        <v>3</v>
-      </c>
-      <c r="J11" s="38">
+      <c r="I11" s="34">
+        <v>3</v>
+      </c>
+      <c r="J11" s="37">
         <v>4</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="18">
         <v>4</v>
       </c>
-      <c r="L11" s="41">
-        <v>3</v>
-      </c>
-      <c r="M11" s="20">
+      <c r="L11" s="18">
+        <v>3</v>
+      </c>
+      <c r="M11" s="15">
         <f t="shared" ref="M11" si="2">-SUM(E11:E13)*$E$15-SUM(H11:H13)*$H$15+I11*$I$15+J11*$J$15+K11*$K$15+L11*$L$15</f>
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="27"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="20"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="8">
         <v>2</v>
       </c>
@@ -1183,15 +1199,15 @@
       <c r="H12" s="11">
         <v>2</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="18"/>
-      <c r="B13" s="28"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="2">
         <v>3</v>
       </c>
@@ -1206,13 +1222,13 @@
       <c r="H13" s="13">
         <v>2</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I13" s="36"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="D14" t="s">
         <v>18</v>
       </c>
@@ -1237,7 +1253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13">
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -1262,19 +1278,96 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="2:12" ht="15" customHeight="1">
+      <c r="B17" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
+  <mergeCells count="31">
+    <mergeCell ref="D17:L23"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B2:B4"/>
@@ -1289,11 +1382,17 @@
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="J8:J10"/>
     <mergeCell ref="J11:J13"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>